<commit_message>
Updated Metformin Screener to include Cancer details and added assertion for the Participant Details page in NV
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
+++ b/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E82395-2F1C-764C-91CE-37B0AF4ABB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBB90E7-8D3C-964B-856F-4478931AF453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="402">
   <si>
     <t>Yes</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>Select Unknown/Unsure if you don't know the date or age of cancer diagnosis</t>
-  </si>
-  <si>
-    <t>Age at Diagnosis</t>
   </si>
   <si>
     <t>Select 0 if diagnosis occurred before age 1.</t>
@@ -1309,12 +1306,42 @@
   <si>
     <t>11/19/2020</t>
   </si>
+  <si>
+    <t>Age at diagnosis</t>
+  </si>
+  <si>
+    <t>Month of diagnosis</t>
+  </si>
+  <si>
+    <t>Year of diagnosis</t>
+  </si>
+  <si>
+    <t>Submit Screen Text1</t>
+  </si>
+  <si>
+    <t>Submit Screen Text2</t>
+  </si>
+  <si>
+    <t>Submit Screen Text3</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Thank you very much. The information you have provided will be reviewed by our study team. You will be contacted by the study team to inform you about the decision regarding whether you are eligible or not eligible to participate in the MILI-NCI study.</t>
+  </si>
+  <si>
+    <t>Please feel free to call at any time if you have any questions regarding this protocol. You may reach out to Payal Khincha, MBBS (payal.khincha@nih.gov, 240.276.7267) or Michele Nehrebecky, NP (nehrebem@mail.nih.gov, 240.858.0000) with questions.</t>
+  </si>
+  <si>
+    <t>Thank you for your willingness to consider joining our research effort. We could not do vital studies like this without the help of dedicated people like you.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1351,6 +1378,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF3A3F51"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1394,7 +1427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1448,6 +1481,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1772,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BDBA15-09FD-FB42-B4F3-2AA9D176499A}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1904,7 +1944,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19">
@@ -2092,7 +2132,7 @@
         <v>66</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="38">
@@ -2102,18 +2142,18 @@
     </row>
     <row r="43" spans="1:2" ht="19">
       <c r="A43" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="171">
       <c r="A44" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19">
@@ -2150,6 +2190,7 @@
       <c r="A49" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="B49" s="15"/>
     </row>
     <row r="50" spans="1:2" ht="19">
       <c r="A50" s="11" t="s">
@@ -2213,7 +2254,7 @@
     </row>
     <row r="58" spans="1:2" ht="19">
       <c r="A58" s="11" t="s">
-        <v>82</v>
+        <v>392</v>
       </c>
       <c r="B58" s="5">
         <v>103</v>
@@ -2221,155 +2262,153 @@
     </row>
     <row r="59" spans="1:2" ht="19">
       <c r="A59" s="11" t="s">
-        <v>83</v>
+        <v>393</v>
       </c>
       <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" ht="19">
       <c r="A60" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" ht="19">
       <c r="A61" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>88</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" ht="19">
       <c r="A62" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B62" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:2" ht="19">
       <c r="A63" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="19">
       <c r="A64" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>91</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" ht="19">
       <c r="A65" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="19">
       <c r="A66" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B66" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="67" spans="1:2" ht="19">
       <c r="A67" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="19">
       <c r="A68" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>391</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" ht="19">
       <c r="A69" s="11" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="19">
       <c r="A70" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>392</v>
+        <v>94</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="19">
       <c r="A71" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>0</v>
+        <v>95</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="19">
       <c r="A72" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B72" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:2" ht="19">
       <c r="A73" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>101</v>
+        <v>379</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="19">
       <c r="A74" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B74" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:2" ht="19">
       <c r="A75" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" ht="19">
       <c r="A76" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19">
       <c r="A77" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B77" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" spans="1:2" ht="19">
+      <c r="A78" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="38">
-      <c r="A78" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" ht="19">
       <c r="A79" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>0</v>
@@ -2377,101 +2416,158 @@
     </row>
     <row r="80" spans="1:2" ht="19">
       <c r="A80" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B80" s="5"/>
-    </row>
-    <row r="81" spans="1:2" ht="19">
+        <v>104</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="38">
       <c r="A81" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="76">
-      <c r="A82" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="95">
-      <c r="A83" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="1:2" ht="19">
+      <c r="A82" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="19">
+      <c r="A83" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" s="5"/>
     </row>
     <row r="84" spans="1:2" ht="19">
       <c r="A84" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="19">
-      <c r="A85" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="76">
+      <c r="A85" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="95">
+      <c r="A86" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="19">
+      <c r="A87" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="19">
-      <c r="A86" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="B86" s="5">
-        <v>1234356758</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="38">
-      <c r="A87" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="19">
       <c r="A88" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>385</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="19">
       <c r="A89" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B89" s="5"/>
-    </row>
-    <row r="90" spans="1:2" ht="19">
+        <v>381</v>
+      </c>
+      <c r="B89" s="5">
+        <v>1234356758</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="38">
       <c r="A90" s="11" t="s">
-        <v>383</v>
+        <v>116</v>
       </c>
       <c r="B90" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="19">
+      <c r="A91" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="38">
-      <c r="A91" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="19">
       <c r="A92" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B92" s="15"/>
+        <v>118</v>
+      </c>
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="1:2" ht="19">
+      <c r="A93" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="38">
+      <c r="A94" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="19">
+      <c r="A95" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B95" s="15"/>
+    </row>
+    <row r="96" spans="1:2" ht="51">
+      <c r="A96" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="B96" s="23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="51">
+      <c r="A97" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="B97" s="23" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="34">
+      <c r="A98" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="B98" s="23" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="17">
+      <c r="A99" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="B99" s="15" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="26">
+      <c r="B100" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2494,97 +2590,97 @@
   <sheetData>
     <row r="2" spans="5:5">
       <c r="E2" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="5:5">
       <c r="E3" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="5:5">
       <c r="E7" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="5:5">
       <c r="E8" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="5:5">
       <c r="E9" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="5:5">
       <c r="E10" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="5:5">
       <c r="E11" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="5:5">
       <c r="E12" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="5:5">
       <c r="E14" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="5:5">
       <c r="E15" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="5:5">
       <c r="E16" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="5:5">
@@ -2592,242 +2688,242 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="5:5">
       <c r="E33" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="5:5">
       <c r="E34" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="5:5">
       <c r="E35" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="5:5">
       <c r="E37" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="5:5">
       <c r="E38" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="5:5">
       <c r="E39" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="5:5">
       <c r="E40" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="5:5">
       <c r="E41" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="5:5">
       <c r="E42" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="5:5">
       <c r="E43" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="5:5">
       <c r="E44" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="5:5">
       <c r="E45" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="5:5">
       <c r="E46" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="5:5">
       <c r="E47" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="5:5">
       <c r="E48" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="5:5">
       <c r="E49" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="5:5">
       <c r="E50" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="5:5">
       <c r="E51" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" spans="5:5">
       <c r="E54" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="5:5">
       <c r="E55" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="5:5">
       <c r="E56" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="57" spans="5:5">
       <c r="E57" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="5:5">
       <c r="E58" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="5:5">
       <c r="E59" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="5:5">
       <c r="E60" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="5:5">
       <c r="E61" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="5:5">
       <c r="E62" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="5:5">
       <c r="E63" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="5:5">
       <c r="E64" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="67" spans="5:5">
       <c r="E67" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="68" spans="5:5">
       <c r="E68" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="5:5">
       <c r="E69" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="70" spans="5:5">
@@ -2838,52 +2934,52 @@
     </row>
     <row r="72" spans="5:5">
       <c r="E72" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="5:5">
       <c r="E74" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75" spans="5:5">
       <c r="E75" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="5:5">
       <c r="E76" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="77" spans="5:5">
       <c r="E77" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="78" spans="5:5">
       <c r="E78" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="5:5">
       <c r="E79" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="5:5">
       <c r="E80" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2909,386 +3005,386 @@
   <sheetData>
     <row r="2" spans="3:9" ht="19">
       <c r="C2" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2,G2)</f>
         <v>public static final String ARE_YOU_COMPLETING_THIS_QUESTIONNAIRE_FOR_SOMEONE_ELSE = "Are you completing this questionnaire for someone else? ";</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="3:9" ht="19">
       <c r="C3" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H20" si="0">CONCATENATE(C3,D3,E3,F3,G3)</f>
         <v>public static final String WHAT_IS_YOUR_NAME = "What is your name? ";</v>
       </c>
       <c r="I3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="3:9" ht="19">
       <c r="C4" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>public static final String FIRST_NAME = "First Name ";</v>
       </c>
       <c r="I4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="19">
       <c r="C5" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>public static final String MIDDLE_INITIAL = "Middle Initial ";</v>
       </c>
       <c r="I5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="19">
       <c r="C6" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>public static final String LAST_NAME = "Last Name ";</v>
       </c>
       <c r="I6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="3:9" ht="19">
       <c r="C7" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>public static final String THE_NEXT_SET_OF_QUESTIONS_WILL_COLLECT_BASIC_INFORMATION_ABOUT_YOU_THE_PARTICIPANT = "The next set of questions will collect basic information about you/the participant. ";</v>
       </c>
       <c r="I7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="3:9" ht="19">
       <c r="C8" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANTS_DATE_OF_BIRTH = "What is your/the participant's date of birth? ";</v>
       </c>
       <c r="I8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="3:9" ht="19">
       <c r="C9" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANTS_SEX = "What is your/the participant's sex? ";</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="3:9" ht="19">
       <c r="C10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" t="s">
         <v>130</v>
       </c>
-      <c r="D10" t="s">
-        <v>131</v>
-      </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>public static final String ARE_YOU_THE_PARTICIPANT_ADOPTED = "Are you/the participant adopted? ";</v>
       </c>
       <c r="I10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="19">
       <c r="C11" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>public static final String IN_WHICH_COUNTRY_DO_YOU_THE_PARTICIPANT_CURRENTLY_LIVE = "In which country do you/the participant currently live? ";</v>
       </c>
       <c r="I11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="19">
       <c r="C12" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>public static final String PLEASE_PROVIDE_THE_MAILING_ADDRESS_WHERE_STUDY_MATERIALS_CAN_BE_SENT_AS_NEEDED = "Please provide the mailing address where study materials can be sent, as needed. ";</v>
       </c>
       <c r="I12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="3:9" ht="19">
       <c r="C13" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>public static final String STREET = "Street ";</v>
       </c>
       <c r="I13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="3:9" ht="19">
       <c r="C14" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>public static final String STREET_2_OPTIONAL = "Street 2 (Optional) ";</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="19">
       <c r="C15" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>public static final String CITY = "City ";</v>
       </c>
       <c r="I15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="19">
       <c r="C16" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>public static final String STATE_ABBREVIATION = "State (Abbreviation) ";</v>
       </c>
       <c r="I16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="3:9" ht="19">
       <c r="C17" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>public static final String ZIP_CODE = "Zip Code ";</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="3:9" s="19" customFormat="1" ht="18">
@@ -3307,67 +3403,67 @@
     </row>
     <row r="21" spans="3:9" ht="19">
       <c r="C21" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H21" t="str">
         <f>CONCATENATE(C21,D21,E21,F21,G21)</f>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS ="What is your/the participant's email address? ";</v>
       </c>
       <c r="I21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="19">
       <c r="C22" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" ref="H22:H40" si="1">CONCATENATE(C22,D22,E22,F22,G22)</f>
         <v>public static final String PLEASE_CONFIRM_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS ="Please confirm your/the participant's email address. ";</v>
       </c>
       <c r="I22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="38">
       <c r="C23" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>40</v>
       </c>
       <c r="G23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
@@ -3375,409 +3471,409 @@
 Please list your/the participant's phone numbers below and include country code. ";</v>
       </c>
       <c r="I23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="3:9" ht="19">
       <c r="C24" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PLEASE_ALSO_SELECT_YOUR_PREFERRED_CONTACT_NUMBER ="Please also select your preferred contact number. ";</v>
       </c>
       <c r="I24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="19">
       <c r="C25" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
         <v>public static final String HOME_PHONE_NUMBER ="Home Phone Number ";</v>
       </c>
       <c r="I25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="3:9" ht="19">
       <c r="C26" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>43</v>
       </c>
       <c r="G26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
         <v>public static final String WORK_PHONE_NUMBER ="Work Phone Number ";</v>
       </c>
       <c r="I26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="3:9" ht="19">
       <c r="C27" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>44</v>
       </c>
       <c r="G27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PREFERRED ="Preferred ";</v>
       </c>
       <c r="I27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="19">
       <c r="C28" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
         <v>public static final String CELL_PHONE_NUMBER ="Cell Phone Number ";</v>
       </c>
       <c r="I28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="3:9" ht="19">
       <c r="C29" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANT'S_RACE_PLEASE_SELECT_ALL_THAT_APPLY ="What is your/the participant's race? Please select all that apply. ";</v>
       </c>
       <c r="I29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="19">
       <c r="C30" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANT'S_ETHNICITY ="What is your/the participant's ethnicity? ";</v>
       </c>
       <c r="I30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="3:9" ht="19">
       <c r="C31" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
         <v>public static final String HAVE_YOU_THE_PARTICIPANT_EVER_PARTICIPATED_IN_A_LIFRAUMENI_SYNDROME_STUDY ="Have you/the participant ever participated in a Li-Fraumeni syndrome study? ";</v>
       </c>
       <c r="I31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="3:9" ht="19">
       <c r="C32" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
         <v>public static final String EG_AT_ANOTHER_MEDICAL_INSTITUTION_UNIVERSITY_GOVERNMENT_AGENCY_OR_OTHER_SITE ="e.g. at another medical institution, university, government agency, or other site ";</v>
       </c>
       <c r="I32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="3:9" ht="38">
       <c r="C33" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PLEASE_SPECIFY_THE_STUDYIES_OR_REGISTRY_GROUPS_REGARDING_PARTICIPATION_IN_OTHER_STUDIES ="Please specify the study(ies) or registry group(s) regarding participation in other studies. ";</v>
       </c>
       <c r="I33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="19">
       <c r="C34" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>52</v>
       </c>
       <c r="G34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
         <v>public static final String DO_YOU_CURRENTLY_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_SCREENING_OR_MANAGEMENT ="Do you currently receive regular Li-Fraumeni syndrome screening or management? ";</v>
       </c>
       <c r="I34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="3:9" ht="38">
       <c r="C35" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>53</v>
       </c>
       <c r="G35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PROVIDE_INFORMATION_ABOUT_THE_INSTITUTION_WHERE_YOU_THE_PARTICIPANT_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_MANAGEMENT ="Provide information about the institution where you/the participant receive regular Li-Fraumeni syndrome management. ";</v>
       </c>
       <c r="I35" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="3:9" ht="19">
       <c r="C36" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F36" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PHYSICIAN_NAME ="Physician Name ";</v>
       </c>
       <c r="I36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="3:9" ht="19">
       <c r="C37" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F37" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
         <v>public static final String INSTITUTION_NAME ="Institution Name ";</v>
       </c>
       <c r="I37" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="19">
       <c r="C38" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
         <v>public static final String CITY_STATE_PROVINCE ="City, State/Province ";</v>
       </c>
       <c r="I38" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="3:9" ht="19">
       <c r="C39" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F39" s="11" t="s">
         <v>57</v>
       </c>
       <c r="G39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PHONE_NUMBERPhone Number ";</v>
       </c>
       <c r="I39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="3:9" ht="57">
       <c r="C40" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>61</v>
       </c>
       <c r="G40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
         <v>public static final String DELIVERY_INFORMATIONTo determine eligibility, we need to collect information about your Li-Fraumeni syndrome diagnosis, genetic testing performed, cancers diagnoses, and medication history. ";</v>
       </c>
       <c r="I40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="18">
@@ -3851,10 +3947,10 @@
   <sheetData>
     <row r="2" spans="7:8" ht="409.6">
       <c r="G2" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3878,290 +3974,290 @@
   <sheetData>
     <row r="2" spans="3:7">
       <c r="C2" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F17" si="0">CONCATENATE(C2,D2,E2)</f>
         <v>public String areYouCompletingThisQuestionnaireForSomeoneElse;</v>
       </c>
       <c r="G2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="3:7">
       <c r="C3" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>public String whatIsYourName;</v>
       </c>
       <c r="G3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>public String firstName;</v>
       </c>
       <c r="G4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="3:7">
       <c r="C5" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>public String middleInitial;</v>
       </c>
       <c r="G5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="3:7">
       <c r="C6" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>public String lastName;</v>
       </c>
       <c r="G6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>public String theNextSetOfQuestionsWillCollectBasicInformationAboutYouTheParticipant;</v>
       </c>
       <c r="G7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="3:7">
       <c r="C8" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>public String whatIsYourTheParticipantsDateOfBirth;</v>
       </c>
       <c r="G8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="3:7">
       <c r="C9" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>public String whatIsYouTheParticipantsSex;</v>
       </c>
       <c r="G9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="3:7">
       <c r="C10" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>public String areYouTheParticipantAdopted;</v>
       </c>
       <c r="G10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="3:7">
       <c r="C11" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>public String inWhichCountryDoYouTheParticipantCurrentlyLive;</v>
       </c>
       <c r="G11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="3:7">
       <c r="C12" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>public String pleaseProvideTheMailingAddressWhereStudyMaterialsCanBeSentAsNeeded;</v>
       </c>
       <c r="G12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="3:7">
       <c r="C13" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v>public String street;</v>
       </c>
       <c r="G13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="3:7">
       <c r="C14" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>public String street2Optional;</v>
       </c>
       <c r="G14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="3:7">
       <c r="C15" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>public String city;</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="3:7">
       <c r="C16" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>public String stateAbbreviation;</v>
       </c>
       <c r="G16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>public String zipCode;</v>
       </c>
       <c r="G17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="3:7" s="19" customFormat="1">
@@ -4173,344 +4269,344 @@
     </row>
     <row r="19" spans="3:7">
       <c r="C19" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
         <v>public String whatIsYourTheParticipantsEmailAddress;</v>
       </c>
       <c r="G19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="3:7">
       <c r="C20" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseConfirmYourTheParticipantsEmailAddress;</v>
       </c>
       <c r="G20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="3:7">
       <c r="C21" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseListYourTheParticipantsPhoneNumbersBelowAndIncludeCountryCode;</v>
       </c>
       <c r="G21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="22" spans="3:7">
       <c r="C22" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseAlsoSelectYourPreferredContactNumber;</v>
       </c>
       <c r="G22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="23" spans="3:7">
       <c r="C23" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
         <v>public String homePhoneNumber;</v>
       </c>
       <c r="G23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="3:7">
       <c r="C24" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
         <v>public String workPhoneNumber;</v>
       </c>
       <c r="G24" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="3:7">
       <c r="C25" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
         <v>public String preferred;</v>
       </c>
       <c r="G25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="3:7">
       <c r="C26" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
         <v>public String cellPhoneNumber;</v>
       </c>
       <c r="G26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="27" spans="3:7">
       <c r="C27" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
         <v>public String whatIsYourTheParticipantsRacePleaseSelectAllThatApply;</v>
       </c>
       <c r="G27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="28" spans="3:7">
       <c r="C28" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
         <v>public String whatIsYourTheParticipantsEthnicity;</v>
       </c>
       <c r="G28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="3:7">
       <c r="C29" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
         <v>public String haveYouTheParticipantEverParticipatedInALiFraumeniSyndromeStudy;</v>
       </c>
       <c r="G29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="3:7">
       <c r="C30" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
         <v>public String egAtAnotherMedicalInstitutionUniversityGovernmentAgencyOrOtherSite;</v>
       </c>
       <c r="G30" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="3:7">
       <c r="C31" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseSpecifyTheStudiesOrRegistryGroupsRegardingParticipationInOtherStudies;</v>
       </c>
       <c r="G31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="3:7">
       <c r="C32" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
         <v>public String doYouCurrentlyReceiveRegularLiFraumeniSyndromeScreeningOrManagement;</v>
       </c>
       <c r="G32" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="33" spans="3:7">
       <c r="C33" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
         <v>public String provideInformationAboutTheInstitutionWhereYou/theParticipantReceiveRegularLiFraumeniSyndromeManagement;</v>
       </c>
       <c r="G33" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="3:7">
       <c r="C34" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
         <v>public String physicianName;</v>
       </c>
       <c r="G34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="3:7">
       <c r="C35" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
         <v>public String institutionName;</v>
       </c>
       <c r="G35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="3:7">
       <c r="C36" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
         <v>public String cityStateProvince;</v>
       </c>
       <c r="G36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="3:7">
       <c r="C37" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
         <v>public String phoneNumber;</v>
       </c>
       <c r="G37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="3:7">
@@ -4543,728 +4639,728 @@
   <sheetData>
     <row r="2" spans="3:8">
       <c r="C2" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2)</f>
         <v>areYouCompletingThisQuestionnaireForSomeoneElse = testDataForMetforminScreener.get(MetforminScreenerConstants.ARE_YOU_COMPLETING_THIS_QUESTIONNAIRE_FOR_SOMEONE_ELSE);</v>
       </c>
       <c r="H2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="3:8">
       <c r="C3" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G17" si="0">CONCATENATE(C3,D3,E3,F3)</f>
         <v>whatIsYourName = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_NAME);</v>
       </c>
       <c r="H3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="3:8">
       <c r="C4" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>firstName = testDataForMetforminScreener.get(MetforminScreenerConstants.FIRST_NAME);</v>
       </c>
       <c r="H4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="3:8">
       <c r="C5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>middleInitial = testDataForMetforminScreener.get(MetforminScreenerConstants.MIDDLE_INITIAL);</v>
       </c>
       <c r="H5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="3:8">
       <c r="C6" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>lastName = testDataForMetforminScreener.get(MetforminScreenerConstants.LAST_NAME);</v>
       </c>
       <c r="H6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="3:8">
       <c r="C7" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" t="s">
         <v>186</v>
-      </c>
-      <c r="E7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" t="s">
-        <v>187</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>theNextSetOfQuestionsWillCollectBasicInformationAboutYouTheParticipant = testDataForMetforminScreener.get(MetforminScreenerConstants.THE_NEXT_SET_OF_QUESTIONS_WILL_COLLECT_BASIC_INFORMATION_ABOUT_YOU_THE_PARTICIPANT);</v>
       </c>
       <c r="H7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="3:8">
       <c r="C8" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" t="s">
         <v>186</v>
-      </c>
-      <c r="E8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" t="s">
-        <v>187</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>whatIsYourTheParticipantsDateOfBirth = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANTS_DATE_OF_BIRTH);</v>
       </c>
       <c r="H8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="3:8">
       <c r="C9" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" t="s">
         <v>186</v>
-      </c>
-      <c r="E9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F9" t="s">
-        <v>187</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>whatIsYouTheParticipantsSex = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANTS_SEX);</v>
       </c>
       <c r="H9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="3:8">
       <c r="C10" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" t="s">
         <v>186</v>
-      </c>
-      <c r="E10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" t="s">
-        <v>187</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>areYouTheParticipantAdopted = testDataForMetforminScreener.get(MetforminScreenerConstants.ARE_YOU_THE_PARTICIPANT_ADOPTED);</v>
       </c>
       <c r="H10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="3:8">
       <c r="C11" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" t="s">
         <v>186</v>
-      </c>
-      <c r="E11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" t="s">
-        <v>187</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>inWhichCountryDoYouTheParticipantCurrentlyLive = testDataForMetforminScreener.get(MetforminScreenerConstants.IN_WHICH_COUNTRY_DO_YOU_THE_PARTICIPANT_CURRENTLY_LIVE);</v>
       </c>
       <c r="H11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="3:8">
       <c r="C12" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
         <v>186</v>
-      </c>
-      <c r="E12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" t="s">
-        <v>187</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>pleaseProvideTheMailingAddressWhereStudyMaterialsCanBeSentAsNeeded = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_PROVIDE_THE_MAILING_ADDRESS_WHERE_STUDY_MATERIALS_CAN_BE_SENT_AS_NEEDED);</v>
       </c>
       <c r="H12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="3:8">
       <c r="C13" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" t="s">
         <v>186</v>
-      </c>
-      <c r="E13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" t="s">
-        <v>187</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>street = testDataForMetforminScreener.get(MetforminScreenerConstants.STREET);</v>
       </c>
       <c r="H13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="3:8">
       <c r="C14" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" t="s">
         <v>186</v>
-      </c>
-      <c r="E14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F14" t="s">
-        <v>187</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>street2Optional = testDataForMetforminScreener.get(MetforminScreenerConstants.STREET_2_OPTIONAL);</v>
       </c>
       <c r="H14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="3:8">
       <c r="C15" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" t="s">
         <v>186</v>
-      </c>
-      <c r="E15" t="s">
-        <v>123</v>
-      </c>
-      <c r="F15" t="s">
-        <v>187</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>city = testDataForMetforminScreener.get(MetforminScreenerConstants.CITY);</v>
       </c>
       <c r="H15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="3:8">
       <c r="C16" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" t="s">
         <v>186</v>
-      </c>
-      <c r="E16" t="s">
-        <v>126</v>
-      </c>
-      <c r="F16" t="s">
-        <v>187</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>stateAbbreviation = testDataForMetforminScreener.get(MetforminScreenerConstants.STATE_ABBREVIATION);</v>
       </c>
       <c r="H16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="3:8">
       <c r="C17" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" t="s">
         <v>186</v>
-      </c>
-      <c r="E17" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" t="s">
-        <v>187</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>zipCode = testDataForMetforminScreener.get(MetforminScreenerConstants.ZIP_CODE);</v>
       </c>
       <c r="H17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="3:8" s="19" customFormat="1"/>
     <row r="19" spans="3:8">
       <c r="C19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" t="s">
         <v>186</v>
-      </c>
-      <c r="E19" t="s">
-        <v>282</v>
-      </c>
-      <c r="F19" t="s">
-        <v>187</v>
       </c>
       <c r="G19" t="str">
         <f>CONCATENATE(C19,D19,E19,F19)</f>
         <v>whatIsYourTheParticipantsEmailAddress = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS);</v>
       </c>
       <c r="H19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="3:8">
       <c r="C20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" t="s">
+        <v>282</v>
+      </c>
+      <c r="F20" t="s">
         <v>186</v>
-      </c>
-      <c r="E20" t="s">
-        <v>283</v>
-      </c>
-      <c r="F20" t="s">
-        <v>187</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ref="G20:G36" si="1">CONCATENATE(C20,D20,E20,F20)</f>
         <v>pleaseConfirmYourTheParticipantsEmailAddress = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_CONFIRM_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS);</v>
       </c>
       <c r="H20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="3:8">
       <c r="C21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" t="s">
+        <v>283</v>
+      </c>
+      <c r="F21" t="s">
         <v>186</v>
-      </c>
-      <c r="E21" t="s">
-        <v>284</v>
-      </c>
-      <c r="F21" t="s">
-        <v>187</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
         <v>pleaseListYourTheParticipantsPhoneNumbersBelowAndIncludeCountryCode = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_LIST_YOUR_THE_PARTICIPANTS_PHONE_NUMBERS_BELOW_AND_INCLUDE_COUNTRY_CODE);</v>
       </c>
       <c r="H21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="3:8">
       <c r="C22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" t="s">
         <v>186</v>
-      </c>
-      <c r="E22" t="s">
-        <v>285</v>
-      </c>
-      <c r="F22" t="s">
-        <v>187</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
         <v>pleaseAlsoSelectYourPreferredContactNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_ALSO_SELECT_YOUR_PREFERRED_CONTACT_NUMBER);</v>
       </c>
       <c r="H22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23" spans="3:8">
       <c r="C23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" t="s">
+        <v>285</v>
+      </c>
+      <c r="F23" t="s">
         <v>186</v>
-      </c>
-      <c r="E23" t="s">
-        <v>286</v>
-      </c>
-      <c r="F23" t="s">
-        <v>187</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
         <v>homePhoneNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.HOME_PHONE_NUMBER);</v>
       </c>
       <c r="H23" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="3:8">
       <c r="C24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D24" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" t="s">
+        <v>286</v>
+      </c>
+      <c r="F24" t="s">
         <v>186</v>
-      </c>
-      <c r="E24" t="s">
-        <v>287</v>
-      </c>
-      <c r="F24" t="s">
-        <v>187</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
         <v>workPhoneNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.WORK_PHONE_NUMBER);</v>
       </c>
       <c r="H24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25" spans="3:8">
       <c r="C25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D25" t="s">
+        <v>185</v>
+      </c>
+      <c r="E25" t="s">
+        <v>211</v>
+      </c>
+      <c r="F25" t="s">
         <v>186</v>
-      </c>
-      <c r="E25" t="s">
-        <v>212</v>
-      </c>
-      <c r="F25" t="s">
-        <v>187</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
         <v>preferred = testDataForMetforminScreener.get(MetforminScreenerConstants.PREFERRED);</v>
       </c>
       <c r="H25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="3:8">
       <c r="C26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D26" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" t="s">
+        <v>287</v>
+      </c>
+      <c r="F26" t="s">
         <v>186</v>
-      </c>
-      <c r="E26" t="s">
-        <v>288</v>
-      </c>
-      <c r="F26" t="s">
-        <v>187</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
         <v>cellPhoneNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.CELL_PHONE_NUMBER);</v>
       </c>
       <c r="H26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="3:8">
       <c r="C27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D27" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F27" t="s">
         <v>186</v>
-      </c>
-      <c r="E27" t="s">
-        <v>289</v>
-      </c>
-      <c r="F27" t="s">
-        <v>187</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
         <v>whatIsYourTheParticipantsRacePleaseSelectAllThatApply = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANT'S_RACE_PLEASE_SELECT_ALL_THAT_APPLY);</v>
       </c>
       <c r="H27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="3:8">
       <c r="C28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D28" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" t="s">
+        <v>289</v>
+      </c>
+      <c r="F28" t="s">
         <v>186</v>
-      </c>
-      <c r="E28" t="s">
-        <v>290</v>
-      </c>
-      <c r="F28" t="s">
-        <v>187</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
         <v>whatIsYourTheParticipantsEthnicity = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANT'S_ETHNICITY);</v>
       </c>
       <c r="H28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="3:8">
       <c r="C29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D29" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" t="s">
+        <v>290</v>
+      </c>
+      <c r="F29" t="s">
         <v>186</v>
-      </c>
-      <c r="E29" t="s">
-        <v>291</v>
-      </c>
-      <c r="F29" t="s">
-        <v>187</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
         <v>haveYouTheParticipantEverParticipatedInALiFraumeniSyndromeStudy = testDataForMetforminScreener.get(MetforminScreenerConstants.HAVE_YOU_THE_PARTICIPANT_EVER_PARTICIPATED_IN_A_LIFRAUMENI_SYNDROME_STUDY);</v>
       </c>
       <c r="H29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="3:8">
       <c r="C30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E30" t="s">
+        <v>291</v>
+      </c>
+      <c r="F30" t="s">
         <v>186</v>
-      </c>
-      <c r="E30" t="s">
-        <v>292</v>
-      </c>
-      <c r="F30" t="s">
-        <v>187</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
         <v>egAtAnotherMedicalInstitutionUniversityGovernmentAgencyOrOtherSite = testDataForMetforminScreener.get(MetforminScreenerConstants.EG_AT_ANOTHER_MEDICAL_INSTITUTION_UNIVERSITY_GOVERNMENT_AGENCY_OR_OTHER_SITE);</v>
       </c>
       <c r="H30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="3:8">
       <c r="C31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D31" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" t="s">
+        <v>292</v>
+      </c>
+      <c r="F31" t="s">
         <v>186</v>
-      </c>
-      <c r="E31" t="s">
-        <v>293</v>
-      </c>
-      <c r="F31" t="s">
-        <v>187</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
         <v>pleaseSpecifyTheStudiesOrRegistryGroupsRegardingParticipationInOtherStudies = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_SPECIFY_THE_STUDYIES_OR_REGISTRY_GROUPS_REGARDING_PARTICIPATION_IN_OTHER_STUDIES);</v>
       </c>
       <c r="H31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="3:8">
       <c r="C32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" t="s">
+        <v>293</v>
+      </c>
+      <c r="F32" t="s">
         <v>186</v>
-      </c>
-      <c r="E32" t="s">
-        <v>294</v>
-      </c>
-      <c r="F32" t="s">
-        <v>187</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
         <v>doYouCurrentlyReceiveRegularLiFraumeniSyndromeScreeningOrManagement = testDataForMetforminScreener.get(MetforminScreenerConstants.DO_YOU_CURRENTLY_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_SCREENING_OR_MANAGEMENT);</v>
       </c>
       <c r="H32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="3:8">
       <c r="C33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" t="s">
+        <v>294</v>
+      </c>
+      <c r="F33" t="s">
         <v>186</v>
-      </c>
-      <c r="E33" t="s">
-        <v>295</v>
-      </c>
-      <c r="F33" t="s">
-        <v>187</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
         <v>provideInformationAboutTheInstitutionWhereYou/theParticipantReceiveRegularLiFraumeniSyndromeManagement = testDataForMetforminScreener.get(MetforminScreenerConstants.PROVIDE_INFORMATION_ABOUT_THE_INSTITUTION_WHERE_YOU_THE_PARTICIPANT_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_MANAGEMENT);</v>
       </c>
       <c r="H33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="3:8">
       <c r="C34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D34" t="s">
+        <v>185</v>
+      </c>
+      <c r="E34" t="s">
+        <v>295</v>
+      </c>
+      <c r="F34" t="s">
         <v>186</v>
-      </c>
-      <c r="E34" t="s">
-        <v>296</v>
-      </c>
-      <c r="F34" t="s">
-        <v>187</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
         <v>physicianName = testDataForMetforminScreener.get(MetforminScreenerConstants.PHYSICIAN_NAME);</v>
       </c>
       <c r="H34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="3:8">
       <c r="C35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D35" t="s">
+        <v>185</v>
+      </c>
+      <c r="E35" t="s">
+        <v>296</v>
+      </c>
+      <c r="F35" t="s">
         <v>186</v>
-      </c>
-      <c r="E35" t="s">
-        <v>297</v>
-      </c>
-      <c r="F35" t="s">
-        <v>187</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
         <v>institutionName = testDataForMetforminScreener.get(MetforminScreenerConstants.INSTITUTION_NAME);</v>
       </c>
       <c r="H35" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="3:8">
       <c r="C36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" t="s">
+        <v>297</v>
+      </c>
+      <c r="F36" t="s">
         <v>186</v>
-      </c>
-      <c r="E36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F36" t="s">
-        <v>187</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
         <v>cityStateProvince = testDataForMetforminScreener.get(MetforminScreenerConstants.CITY_STATE_PROVINCE);</v>
       </c>
       <c r="H36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="3:8">
       <c r="C37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed extra spaces in export
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
+++ b/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBB90E7-8D3C-964B-856F-4478931AF453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF6D74-7D3C-CE4C-B73A-B92A9A52FA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="740" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="MetforminScreenerScenario1" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="405">
   <si>
     <t>Yes</t>
   </si>
@@ -1335,6 +1335,15 @@
   </si>
   <si>
     <t>Thank you for your willingness to consider joining our research effort. We could not do vital studies like this without the help of dedicated people like you.</t>
+  </si>
+  <si>
+    <t>Proxy First Name</t>
+  </si>
+  <si>
+    <t>Proxy Middle Initial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proxy Last Name</t>
   </si>
 </sst>
 </file>
@@ -1812,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BDBA15-09FD-FB42-B4F3-2AA9D176499A}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1873,564 +1882,559 @@
     </row>
     <row r="7" spans="1:2" ht="19">
       <c r="A7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="5"/>
+        <v>402</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="19">
       <c r="A8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>37</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:2" ht="19">
       <c r="A9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:2" ht="19">
       <c r="A10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" ht="19">
       <c r="A11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19">
       <c r="A12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="19">
       <c r="A13" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19">
       <c r="A14" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19">
       <c r="A15" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:2" ht="19">
       <c r="A16" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>385</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19">
       <c r="A17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5">
-        <v>80439</v>
+        <v>30</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19">
       <c r="A18" s="11" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19">
       <c r="A19" s="11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="38">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="19">
       <c r="A20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B20" s="5">
+        <v>80439</v>
+      </c>
     </row>
     <row r="21" spans="1:2" ht="19">
       <c r="A21" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="19">
       <c r="A22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="19">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="38">
       <c r="A23" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="5">
-        <v>2341234567</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" ht="19">
       <c r="A24" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" ht="19">
       <c r="A25" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" s="5">
-        <v>3456784567</v>
+        <v>1234567890</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19">
       <c r="A26" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>4</v>
+        <v>43</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2341234567</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19">
       <c r="A27" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" ht="19">
       <c r="A28" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="B28" s="5">
+        <v>3456784567</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19">
       <c r="A29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" ht="38">
+        <v>46</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="19">
       <c r="A30" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19">
       <c r="A31" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="38">
+    <row r="32" spans="1:2" ht="19">
       <c r="A32" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B32" s="5"/>
     </row>
-    <row r="33" spans="1:2" ht="19">
+    <row r="33" spans="1:2" ht="38">
       <c r="A33" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19">
       <c r="A34" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="38">
       <c r="A35" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" ht="19">
       <c r="A36" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="5">
-        <v>2104566789</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="57">
+        <v>54</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19">
       <c r="A37" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="38" spans="1:2" ht="19">
       <c r="A38" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19">
       <c r="A39" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="19">
+        <v>57</v>
+      </c>
+      <c r="B39" s="5">
+        <v>2104566789</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="57">
       <c r="A40" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" ht="19">
       <c r="A41" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19">
       <c r="A42" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19">
       <c r="A43" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="171">
+        <v>64</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19">
       <c r="A44" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="19">
+        <v>66</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="38">
       <c r="A45" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19">
       <c r="A46" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="171">
+      <c r="A47" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="19">
+      <c r="A48" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="19">
+      <c r="A49" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="19">
-      <c r="A47" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="38">
-      <c r="A48" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="5"/>
-    </row>
-    <row r="49" spans="1:2" ht="57">
-      <c r="A49" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="15"/>
     </row>
     <row r="50" spans="1:2" ht="19">
       <c r="A50" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" s="5"/>
-    </row>
-    <row r="51" spans="1:2" ht="19">
+        <v>70</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="38">
       <c r="A51" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="19">
-      <c r="A52" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>75</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="1:2" ht="57">
+      <c r="A52" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="15"/>
     </row>
     <row r="53" spans="1:2" ht="19">
       <c r="A53" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" ht="19">
       <c r="A54" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19">
       <c r="A55" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19">
       <c r="A56" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>6</v>
+        <v>76</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19">
       <c r="A57" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="58" spans="1:2" ht="19">
       <c r="A58" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="B58" s="5">
-        <v>103</v>
+        <v>77</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19">
       <c r="A59" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="B59" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="60" spans="1:2" ht="19">
       <c r="A60" s="11" t="s">
-        <v>394</v>
+        <v>81</v>
       </c>
       <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" ht="19">
       <c r="A61" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" s="5"/>
+        <v>392</v>
+      </c>
+      <c r="B61" s="5">
+        <v>103</v>
+      </c>
     </row>
     <row r="62" spans="1:2" ht="19">
       <c r="A62" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" ht="19">
       <c r="A63" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" ht="19">
       <c r="A64" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" ht="19">
       <c r="A65" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="19">
       <c r="A66" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19">
       <c r="A67" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>93</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" ht="19">
       <c r="A68" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="69" spans="1:2" ht="19">
       <c r="A69" s="11" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="19">
       <c r="A70" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="19">
       <c r="A71" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>390</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" ht="19">
       <c r="A72" s="11" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="19">
       <c r="A73" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>391</v>
+        <v>94</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="19">
       <c r="A74" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>0</v>
+        <v>95</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="19">
       <c r="A75" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B75" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:2" ht="19">
       <c r="A76" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>100</v>
+        <v>379</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19">
       <c r="A77" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B77" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:2" ht="19">
       <c r="A78" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" ht="19">
       <c r="A79" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="19">
       <c r="A80" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B80" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="1:2" ht="19">
+      <c r="A81" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="38">
-      <c r="A81" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" ht="19">
       <c r="A82" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>0</v>
@@ -2438,136 +2442,158 @@
     </row>
     <row r="83" spans="1:2" ht="19">
       <c r="A83" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="38">
+      <c r="A84" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" spans="1:2" ht="19">
+      <c r="A85" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="19">
+      <c r="A86" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B83" s="5"/>
-    </row>
-    <row r="84" spans="1:2" ht="19">
-      <c r="A84" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="76">
-      <c r="A85" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="95">
-      <c r="A86" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>111</v>
-      </c>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" ht="19">
       <c r="A87" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="76">
+      <c r="A88" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="95">
+      <c r="A89" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="19">
+      <c r="A90" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B90" s="5" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="19">
-      <c r="A88" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="19">
-      <c r="A89" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="B89" s="5">
-        <v>1234356758</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="38">
-      <c r="A90" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="19">
       <c r="A91" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>384</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="19">
       <c r="A92" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B92" s="5"/>
-    </row>
-    <row r="93" spans="1:2" ht="19">
+        <v>381</v>
+      </c>
+      <c r="B92" s="5">
+        <v>1234356758</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="38">
       <c r="A93" s="11" t="s">
-        <v>382</v>
+        <v>116</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="19">
       <c r="A94" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="19">
       <c r="A95" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" spans="1:2" ht="19">
+      <c r="A96" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="38">
+      <c r="A97" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="19">
+      <c r="A98" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B95" s="15"/>
-    </row>
-    <row r="96" spans="1:2" ht="51">
-      <c r="A96" s="24" t="s">
+      <c r="B98" s="15"/>
+    </row>
+    <row r="99" spans="1:2" ht="51">
+      <c r="A99" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="B96" s="23" t="s">
+      <c r="B99" s="23" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="51">
-      <c r="A97" s="24" t="s">
+    <row r="100" spans="1:2" ht="51">
+      <c r="A100" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="B97" s="23" t="s">
+      <c r="B100" s="23" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="34">
-      <c r="A98" s="24" t="s">
+    <row r="101" spans="1:2" ht="34">
+      <c r="A101" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="B98" s="23" t="s">
+      <c r="B101" s="23" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="17">
-      <c r="A99" s="24" t="s">
+    <row r="102" spans="1:2" ht="17">
+      <c r="A102" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B102" s="15" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="26">
-      <c r="B100" s="22"/>
+    <row r="103" spans="1:2" ht="26">
+      <c r="B103" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the Assertions of the Metformin Screener in Participant details page of the NativeView
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
+++ b/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF6D74-7D3C-CE4C-B73A-B92A9A52FA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE0CA8-DBD4-BF41-A6F8-FF79E32A534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="MetforminScreenerScenario1" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet8" sheetId="11" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet9" sheetId="12" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="9" r:id="rId6"/>
-    <sheet name="MetforminScreenerScenario2" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="Sheet8" sheetId="11" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet9" sheetId="12" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="9" r:id="rId7"/>
+    <sheet name="MetforminScreenerScenario2" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="429">
   <si>
     <t>Yes</t>
   </si>
@@ -150,9 +151,6 @@
   </si>
   <si>
     <t>Historic Downtown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> San Francisco</t>
   </si>
   <si>
     <t>05/31/1956</t>
@@ -219,13 +217,7 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t xml:space="preserve"> Physician Name Test</t>
-  </si>
-  <si>
     <t>Institution Name Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> San Francisco, California 80439</t>
   </si>
   <si>
     <t>To determine eligibility, we need to collect information about your Li-Fraumeni syndrome diagnosis, genetic testing performed, cancers diagnoses, and medication history.</t>
@@ -1280,9 +1272,6 @@
     <t>Receive genetic testing</t>
   </si>
   <si>
-    <t>CL</t>
-  </si>
-  <si>
     <t>Delivery HelpText</t>
   </si>
   <si>
@@ -1340,17 +1329,101 @@
     <t>Proxy First Name</t>
   </si>
   <si>
-    <t>Proxy Middle Initial</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Proxy Last Name</t>
+    <t>Proxy Last Name</t>
+  </si>
+  <si>
+    <t>Vital Status</t>
+  </si>
+  <si>
+    <t>Alive</t>
+  </si>
+  <si>
+    <t>Calculated Age</t>
+  </si>
+  <si>
+    <t>What is your relationship to the participant?</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Are you the legal guardian of this person?</t>
+  </si>
+  <si>
+    <t>Does the participant need legal representation?</t>
+  </si>
+  <si>
+    <t>Registration Email</t>
+  </si>
+  <si>
+    <t>Metformin1Test1@yopmail.com</t>
+  </si>
+  <si>
+    <t>Please list your/the participant's phone numbers below and include country code.</t>
+  </si>
+  <si>
+    <t>San Francisco, California 80439</t>
+  </si>
+  <si>
+    <t>Physician Name Test</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Proxy Contact Street Address</t>
+  </si>
+  <si>
+    <t>Proxy Contact Street Address 2 (optional)</t>
+  </si>
+  <si>
+    <t>Proxy Contact City</t>
+  </si>
+  <si>
+    <t>Proxy Contact State</t>
+  </si>
+  <si>
+    <t>Proxy Contact Zipcode</t>
+  </si>
+  <si>
+    <t>Proxy Contact Country</t>
+  </si>
+  <si>
+    <t>Proxy Contact Email</t>
+  </si>
+  <si>
+    <t>Proxy Contact Home Phone</t>
+  </si>
+  <si>
+    <t>Proxy Contact Cell Phone</t>
+  </si>
+  <si>
+    <t>Proxy Contact Work Phone</t>
+  </si>
+  <si>
+    <t>Proxy Preferred Phone</t>
+  </si>
+  <si>
+    <t>Proxy Middle Name</t>
+  </si>
+  <si>
+    <t>Preferred Contact</t>
+  </si>
+  <si>
+    <t>work_phone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1387,12 +1460,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF3A3F51"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1436,7 +1503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1490,13 +1557,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1821,10 +1881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BDBA15-09FD-FB42-B4F3-2AA9D176499A}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1882,18 +1942,18 @@
     </row>
     <row r="7" spans="1:2" ht="19">
       <c r="A7" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19">
       <c r="A8" s="11" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:2" ht="19">
       <c r="A9" s="11" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B9" s="5"/>
     </row>
@@ -1908,7 +1968,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19">
@@ -1962,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19">
@@ -1970,7 +2030,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>385</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19">
@@ -1986,32 +2046,32 @@
         <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19">
       <c r="A22" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="19">
       <c r="A23" s="11" t="s">
-        <v>40</v>
+        <v>411</v>
       </c>
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" ht="19">
       <c r="A24" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" ht="19">
       <c r="A25" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="5">
         <v>1234567890</v>
@@ -2019,7 +2079,7 @@
     </row>
     <row r="26" spans="1:2" ht="19">
       <c r="A26" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="5">
         <v>2341234567</v>
@@ -2027,13 +2087,15 @@
     </row>
     <row r="27" spans="1:2" ht="19">
       <c r="A27" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2341234567</v>
+      </c>
     </row>
     <row r="28" spans="1:2" ht="19">
       <c r="A28" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="5">
         <v>3456784567</v>
@@ -2041,7 +2103,7 @@
     </row>
     <row r="29" spans="1:2" ht="19">
       <c r="A29" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>4</v>
@@ -2049,7 +2111,7 @@
     </row>
     <row r="30" spans="1:2" ht="19">
       <c r="A30" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>3</v>
@@ -2057,7 +2119,7 @@
     </row>
     <row r="31" spans="1:2" ht="19">
       <c r="A31" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>0</v>
@@ -2065,21 +2127,21 @@
     </row>
     <row r="32" spans="1:2" ht="19">
       <c r="A32" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:2" ht="25" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" ht="38">
-      <c r="A33" s="11" t="s">
+      <c r="B33" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19">
       <c r="A34" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>0</v>
@@ -2087,51 +2149,51 @@
     </row>
     <row r="35" spans="1:2" ht="38">
       <c r="A35" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" ht="19">
       <c r="A36" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>58</v>
+        <v>413</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19">
       <c r="A37" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19">
       <c r="A38" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>60</v>
+        <v>412</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19">
       <c r="A39" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" s="5">
         <v>2104566789</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="57">
+    <row r="40" spans="1:2" ht="40" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B40" s="5"/>
     </row>
     <row r="41" spans="1:2" ht="19">
       <c r="A41" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>0</v>
@@ -2139,7 +2201,7 @@
     </row>
     <row r="42" spans="1:2" ht="19">
       <c r="A42" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>0</v>
@@ -2147,44 +2209,44 @@
     </row>
     <row r="43" spans="1:2" ht="19">
       <c r="A43" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19">
       <c r="A44" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="38">
       <c r="A45" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19">
       <c r="A46" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>389</v>
+        <v>385</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="171">
       <c r="A47" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>388</v>
+        <v>382</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19">
       <c r="A48" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>0</v>
@@ -2192,7 +2254,7 @@
     </row>
     <row r="49" spans="1:2" ht="19">
       <c r="A49" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>0</v>
@@ -2200,7 +2262,7 @@
     </row>
     <row r="50" spans="1:2" ht="19">
       <c r="A50" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>0</v>
@@ -2208,65 +2270,65 @@
     </row>
     <row r="51" spans="1:2" ht="38">
       <c r="A51" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" ht="57">
-      <c r="A52" s="4" t="s">
-        <v>72</v>
+      <c r="A52" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="B52" s="15"/>
     </row>
     <row r="53" spans="1:2" ht="19">
       <c r="A53" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" ht="19">
       <c r="A54" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19">
       <c r="A55" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19">
       <c r="A56" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19">
       <c r="A57" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="19">
       <c r="A58" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19">
       <c r="A59" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>6</v>
@@ -2274,13 +2336,13 @@
     </row>
     <row r="60" spans="1:2" ht="19">
       <c r="A60" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" ht="19">
       <c r="A61" s="11" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B61" s="5">
         <v>103</v>
@@ -2288,25 +2350,25 @@
     </row>
     <row r="62" spans="1:2" ht="19">
       <c r="A62" s="11" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" ht="19">
       <c r="A63" s="11" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B63" s="5"/>
     </row>
     <row r="64" spans="1:2" ht="19">
       <c r="A64" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" ht="19">
       <c r="A65" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>0</v>
@@ -2314,45 +2376,45 @@
     </row>
     <row r="66" spans="1:2" ht="19">
       <c r="A66" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19">
       <c r="A67" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" ht="19">
       <c r="A68" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="19">
       <c r="A69" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="19">
       <c r="A70" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="19">
       <c r="A71" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B71" s="5"/>
     </row>
@@ -2366,7 +2428,7 @@
     </row>
     <row r="73" spans="1:2" ht="19">
       <c r="A73" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>0</v>
@@ -2374,15 +2436,15 @@
     </row>
     <row r="74" spans="1:2" ht="19">
       <c r="A74" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="19">
       <c r="A75" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>0</v>
@@ -2390,15 +2452,15 @@
     </row>
     <row r="76" spans="1:2" ht="19">
       <c r="A76" s="11" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19">
       <c r="A77" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>0</v>
@@ -2406,202 +2468,350 @@
     </row>
     <row r="78" spans="1:2" ht="19">
       <c r="A78" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" ht="19">
       <c r="A79" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="19">
       <c r="A80" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B80" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" spans="1:2" ht="19">
       <c r="A81" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B81" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="19">
       <c r="A82" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B82" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="19">
       <c r="A83" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B83" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="38">
       <c r="A84" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B84" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" ht="19">
       <c r="A85" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B85" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="19">
       <c r="A86" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B86" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="B86" s="4"/>
     </row>
     <row r="87" spans="1:2" ht="19">
       <c r="A87" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="76">
+      <c r="A88" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="95">
+      <c r="A89" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="76">
-      <c r="A88" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="95">
-      <c r="A89" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="19">
       <c r="A90" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="19">
       <c r="A91" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="19">
       <c r="A92" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="B92" s="5">
+        <v>378</v>
+      </c>
+      <c r="B92" s="4">
         <v>1234356758</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="38">
       <c r="A93" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B93" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="19">
       <c r="A94" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>384</v>
+        <v>114</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="19">
       <c r="A95" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B95" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="B95" s="4"/>
     </row>
     <row r="96" spans="1:2" ht="19">
       <c r="A96" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>383</v>
+        <v>379</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="38">
       <c r="A97" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="19">
       <c r="A98" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B98" s="15"/>
-    </row>
-    <row r="99" spans="1:2" ht="51">
-      <c r="A99" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" s="4"/>
+    </row>
+    <row r="99" spans="1:2" ht="76">
+      <c r="A99" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B99" s="23" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="51">
-      <c r="A100" s="24" t="s">
+    </row>
+    <row r="100" spans="1:2" ht="95">
+      <c r="A100" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B100" s="23" t="s">
+    </row>
+    <row r="101" spans="1:2" ht="57">
+      <c r="A101" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="19">
+      <c r="A102" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="19">
+      <c r="A103" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="19">
+      <c r="A104" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="19">
+      <c r="A105" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:2" ht="19">
+      <c r="A106" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="19">
+      <c r="A107" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="19">
+      <c r="A108" s="11" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" ht="34">
-      <c r="A101" s="24" t="s">
-        <v>397</v>
-      </c>
-      <c r="B101" s="23" t="s">
+      <c r="B108" s="5" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="17">
-      <c r="A102" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="B102" s="15" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="26">
-      <c r="B103" s="22"/>
+    <row r="109" spans="1:2" ht="19">
+      <c r="A109" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="B109" s="5"/>
+    </row>
+    <row r="110" spans="1:2" ht="19">
+      <c r="A110" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="B110" s="5"/>
+    </row>
+    <row r="111" spans="1:2" ht="19">
+      <c r="A111" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="1:2" ht="19">
+      <c r="A112" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="B112" s="5"/>
+    </row>
+    <row r="113" spans="1:2" ht="19">
+      <c r="A113" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="B113" s="5"/>
+    </row>
+    <row r="114" spans="1:2" ht="19">
+      <c r="A114" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B114" s="15"/>
+    </row>
+    <row r="115" spans="1:2" ht="19">
+      <c r="A115" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="B115" s="15"/>
+    </row>
+    <row r="116" spans="1:2" ht="19">
+      <c r="A116" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="B116" s="15"/>
+    </row>
+    <row r="117" spans="1:2" ht="19">
+      <c r="A117" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="B117" s="15"/>
+    </row>
+    <row r="118" spans="1:2" ht="19">
+      <c r="A118" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="B118" s="15"/>
+    </row>
+    <row r="119" spans="1:2" ht="19">
+      <c r="A119" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="B119" s="15"/>
+    </row>
+    <row r="120" spans="1:2" ht="19">
+      <c r="A120" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>428</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B106" r:id="rId1" xr:uid="{79ECE5D9-FE27-534A-9CE9-220483AFFCAE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89481F3-DE1D-084D-8820-B9A4FEFE8064}">
+  <dimension ref="F3:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="6" max="6" width="59.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="6:6" ht="18">
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="6:6" ht="152">
+      <c r="F4" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8893135-DC7A-C241-A6F6-938ADF884C45}">
   <dimension ref="E2:E81"/>
   <sheetViews>
@@ -2616,97 +2826,97 @@
   <sheetData>
     <row r="2" spans="5:5">
       <c r="E2" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="5:5">
       <c r="E3" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="5:5">
       <c r="E7" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="5:5">
       <c r="E8" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="5:5">
       <c r="E9" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="5:5">
       <c r="E10" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="5:5">
       <c r="E11" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="5:5">
       <c r="E12" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="5:5">
       <c r="E14" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="5:5">
       <c r="E15" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="5:5">
       <c r="E16" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="5:5">
@@ -2714,242 +2924,242 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="5:5">
       <c r="E30" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="5:5">
       <c r="E31" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="5:5">
       <c r="E33" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="5:5">
       <c r="E34" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="5:5">
       <c r="E35" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="5:5">
       <c r="E37" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="5:5">
       <c r="E38" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="5:5">
       <c r="E39" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="5:5">
       <c r="E40" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="5:5">
       <c r="E41" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="5:5">
       <c r="E42" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="5:5">
       <c r="E43" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="5:5">
       <c r="E44" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="5:5">
       <c r="E45" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="5:5">
       <c r="E46" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="5:5">
       <c r="E47" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="5:5">
       <c r="E48" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="5:5">
       <c r="E49" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="5:5">
       <c r="E50" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="5:5">
       <c r="E51" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" spans="5:5">
       <c r="E54" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="5:5">
       <c r="E55" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="5:5">
       <c r="E56" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="5:5">
       <c r="E57" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="5:5">
       <c r="E58" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="5:5">
       <c r="E59" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="5:5">
       <c r="E60" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="5:5">
       <c r="E61" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="5:5">
       <c r="E62" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="5:5">
       <c r="E63" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="64" spans="5:5">
       <c r="E64" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="5:5">
       <c r="E67" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="5:5">
       <c r="E68" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="5:5">
       <c r="E69" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="5:5">
@@ -2960,52 +3170,52 @@
     </row>
     <row r="72" spans="5:5">
       <c r="E72" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="5:5">
       <c r="E74" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="5:5">
       <c r="E75" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="5:5">
       <c r="E76" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="77" spans="5:5">
       <c r="E77" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="5:5">
       <c r="E78" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="79" spans="5:5">
       <c r="E79" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="5:5">
       <c r="E80" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3014,7 +3224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3BD33-B5B5-034F-9377-39C67236667B}">
   <dimension ref="C2:I51"/>
   <sheetViews>
@@ -3031,386 +3241,386 @@
   <sheetData>
     <row r="2" spans="3:9" ht="19">
       <c r="C2" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2,G2)</f>
         <v>public static final String ARE_YOU_COMPLETING_THIS_QUESTIONNAIRE_FOR_SOMEONE_ELSE = "Are you completing this questionnaire for someone else? ";</v>
       </c>
       <c r="I2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="3:9" ht="19">
       <c r="C3" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H20" si="0">CONCATENATE(C3,D3,E3,F3,G3)</f>
         <v>public static final String WHAT_IS_YOUR_NAME = "What is your name? ";</v>
       </c>
       <c r="I3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="3:9" ht="19">
       <c r="C4" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>public static final String FIRST_NAME = "First Name ";</v>
       </c>
       <c r="I4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="19">
       <c r="C5" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>public static final String MIDDLE_INITIAL = "Middle Initial ";</v>
       </c>
       <c r="I5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="19">
       <c r="C6" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>public static final String LAST_NAME = "Last Name ";</v>
       </c>
       <c r="I6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="3:9" ht="19">
       <c r="C7" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>public static final String THE_NEXT_SET_OF_QUESTIONS_WILL_COLLECT_BASIC_INFORMATION_ABOUT_YOU_THE_PARTICIPANT = "The next set of questions will collect basic information about you/the participant. ";</v>
       </c>
       <c r="I7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="3:9" ht="19">
       <c r="C8" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANTS_DATE_OF_BIRTH = "What is your/the participant's date of birth? ";</v>
       </c>
       <c r="I8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="3:9" ht="19">
       <c r="C9" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANTS_SEX = "What is your/the participant's sex? ";</v>
       </c>
       <c r="I9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="3:9" ht="19">
       <c r="C10" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>public static final String ARE_YOU_THE_PARTICIPANT_ADOPTED = "Are you/the participant adopted? ";</v>
       </c>
       <c r="I10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="19">
       <c r="C11" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>public static final String IN_WHICH_COUNTRY_DO_YOU_THE_PARTICIPANT_CURRENTLY_LIVE = "In which country do you/the participant currently live? ";</v>
       </c>
       <c r="I11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="19">
       <c r="C12" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>public static final String PLEASE_PROVIDE_THE_MAILING_ADDRESS_WHERE_STUDY_MATERIALS_CAN_BE_SENT_AS_NEEDED = "Please provide the mailing address where study materials can be sent, as needed. ";</v>
       </c>
       <c r="I12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="3:9" ht="19">
       <c r="C13" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>public static final String STREET = "Street ";</v>
       </c>
       <c r="I13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="3:9" ht="19">
       <c r="C14" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>public static final String STREET_2_OPTIONAL = "Street 2 (Optional) ";</v>
       </c>
       <c r="I14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="19">
       <c r="C15" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>public static final String CITY = "City ";</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="19">
       <c r="C16" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" t="s">
         <v>125</v>
-      </c>
-      <c r="E16" t="s">
-        <v>128</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>public static final String STATE_ABBREVIATION = "State (Abbreviation) ";</v>
       </c>
       <c r="I16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="3:9" ht="19">
       <c r="C17" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>public static final String ZIP_CODE = "Zip Code ";</v>
       </c>
       <c r="I17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="3:9" s="19" customFormat="1" ht="18">
@@ -3429,67 +3639,67 @@
     </row>
     <row r="21" spans="3:9" ht="19">
       <c r="C21" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H21" t="str">
         <f>CONCATENATE(C21,D21,E21,F21,G21)</f>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS ="What is your/the participant's email address? ";</v>
       </c>
       <c r="I21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="19">
       <c r="C22" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E22" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" ref="H22:H40" si="1">CONCATENATE(C22,D22,E22,F22,G22)</f>
         <v>public static final String PLEASE_CONFIRM_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS ="Please confirm your/the participant's email address. ";</v>
       </c>
       <c r="I22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="38">
       <c r="C23" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
@@ -3497,409 +3707,409 @@
 Please list your/the participant's phone numbers below and include country code. ";</v>
       </c>
       <c r="I23" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="3:9" ht="19">
       <c r="C24" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E24" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PLEASE_ALSO_SELECT_YOUR_PREFERRED_CONTACT_NUMBER ="Please also select your preferred contact number. ";</v>
       </c>
       <c r="I24" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="19">
       <c r="C25" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E25" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
         <v>public static final String HOME_PHONE_NUMBER ="Home Phone Number ";</v>
       </c>
       <c r="I25" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="3:9" ht="19">
       <c r="C26" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E26" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
         <v>public static final String WORK_PHONE_NUMBER ="Work Phone Number ";</v>
       </c>
       <c r="I26" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="3:9" ht="19">
       <c r="C27" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E27" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PREFERRED ="Preferred ";</v>
       </c>
       <c r="I27" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="3:9" ht="19">
       <c r="C28" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E28" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
         <v>public static final String CELL_PHONE_NUMBER ="Cell Phone Number ";</v>
       </c>
       <c r="I28" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="3:9" ht="19">
       <c r="C29" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D29" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E29" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANT'S_RACE_PLEASE_SELECT_ALL_THAT_APPLY ="What is your/the participant's race? Please select all that apply. ";</v>
       </c>
       <c r="I29" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="3:9" ht="19">
       <c r="C30" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E30" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
         <v>public static final String WHAT_IS_YOUR_THE_PARTICIPANT'S_ETHNICITY ="What is your/the participant's ethnicity? ";</v>
       </c>
       <c r="I30" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="3:9" ht="19">
       <c r="C31" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
         <v>public static final String HAVE_YOU_THE_PARTICIPANT_EVER_PARTICIPATED_IN_A_LIFRAUMENI_SYNDROME_STUDY ="Have you/the participant ever participated in a Li-Fraumeni syndrome study? ";</v>
       </c>
       <c r="I31" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="3:9" ht="19">
       <c r="C32" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D32" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E32" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
         <v>public static final String EG_AT_ANOTHER_MEDICAL_INSTITUTION_UNIVERSITY_GOVERNMENT_AGENCY_OR_OTHER_SITE ="e.g. at another medical institution, university, government agency, or other site ";</v>
       </c>
       <c r="I32" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="33" spans="3:9" ht="38">
       <c r="C33" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D33" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E33" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G33" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PLEASE_SPECIFY_THE_STUDYIES_OR_REGISTRY_GROUPS_REGARDING_PARTICIPATION_IN_OTHER_STUDIES ="Please specify the study(ies) or registry group(s) regarding participation in other studies. ";</v>
       </c>
       <c r="I33" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="19">
       <c r="C34" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E34" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
         <v>public static final String DO_YOU_CURRENTLY_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_SCREENING_OR_MANAGEMENT ="Do you currently receive regular Li-Fraumeni syndrome screening or management? ";</v>
       </c>
       <c r="I34" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="35" spans="3:9" ht="38">
       <c r="C35" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D35" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E35" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PROVIDE_INFORMATION_ABOUT_THE_INSTITUTION_WHERE_YOU_THE_PARTICIPANT_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_MANAGEMENT ="Provide information about the institution where you/the participant receive regular Li-Fraumeni syndrome management. ";</v>
       </c>
       <c r="I35" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="3:9" ht="19">
       <c r="C36" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E36" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PHYSICIAN_NAME ="Physician Name ";</v>
       </c>
       <c r="I36" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="3:9" ht="19">
       <c r="C37" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D37" t="s">
+        <v>293</v>
+      </c>
+      <c r="E37" t="s">
         <v>296</v>
       </c>
-      <c r="E37" t="s">
-        <v>299</v>
-      </c>
       <c r="F37" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
         <v>public static final String INSTITUTION_NAME ="Institution Name ";</v>
       </c>
       <c r="I37" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="3:9" ht="19">
       <c r="C38" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E38" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
         <v>public static final String CITY_STATE_PROVINCE ="City, State/Province ";</v>
       </c>
       <c r="I38" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="3:9" ht="19">
       <c r="C39" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D39" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
         <v>public static final String PHONE_NUMBERPhone Number ";</v>
       </c>
       <c r="I39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="3:9" ht="57">
       <c r="C40" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G40" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
         <v>public static final String DELIVERY_INFORMATIONTo determine eligibility, we need to collect information about your Li-Fraumeni syndrome diagnosis, genetic testing performed, cancers diagnoses, and medication history. ";</v>
       </c>
       <c r="I40" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="3:9" ht="18">
@@ -3961,7 +4171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D26075-03E2-6D49-B34D-6A66EA88B4F3}">
   <dimension ref="G2:H2"/>
   <sheetViews>
@@ -3973,10 +4183,10 @@
   <sheetData>
     <row r="2" spans="7:8" ht="409.6">
       <c r="G2" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3984,7 +4194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6723C2-64BA-2E4A-9742-DB943F1C4B65}">
   <dimension ref="C2:G38"/>
   <sheetViews>
@@ -4000,290 +4210,290 @@
   <sheetData>
     <row r="2" spans="3:7">
       <c r="C2" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F17" si="0">CONCATENATE(C2,D2,E2)</f>
         <v>public String areYouCompletingThisQuestionnaireForSomeoneElse;</v>
       </c>
       <c r="G2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="3:7">
       <c r="C3" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>public String whatIsYourName;</v>
       </c>
       <c r="G3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>public String firstName;</v>
       </c>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="3:7">
       <c r="C5" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>public String middleInitial;</v>
       </c>
       <c r="G5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="3:7">
       <c r="C6" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>public String lastName;</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="3:7">
       <c r="C7" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>public String theNextSetOfQuestionsWillCollectBasicInformationAboutYouTheParticipant;</v>
       </c>
       <c r="G7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="3:7">
       <c r="C8" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>public String whatIsYourTheParticipantsDateOfBirth;</v>
       </c>
       <c r="G8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="3:7">
       <c r="C9" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>public String whatIsYouTheParticipantsSex;</v>
       </c>
       <c r="G9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="3:7">
       <c r="C10" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>public String areYouTheParticipantAdopted;</v>
       </c>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="3:7">
       <c r="C11" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>public String inWhichCountryDoYouTheParticipantCurrentlyLive;</v>
       </c>
       <c r="G11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="3:7">
       <c r="C12" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>public String pleaseProvideTheMailingAddressWhereStudyMaterialsCanBeSentAsNeeded;</v>
       </c>
       <c r="G12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="3:7">
       <c r="C13" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v>public String street;</v>
       </c>
       <c r="G13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="3:7">
       <c r="C14" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>public String street2Optional;</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="3:7">
       <c r="C15" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>public String city;</v>
       </c>
       <c r="G15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="3:7">
       <c r="C16" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>public String stateAbbreviation;</v>
       </c>
       <c r="G16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="3:7">
       <c r="C17" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>public String zipCode;</v>
       </c>
       <c r="G17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="3:7" s="19" customFormat="1">
@@ -4295,344 +4505,344 @@
     </row>
     <row r="19" spans="3:7">
       <c r="C19" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
         <v>public String whatIsYourTheParticipantsEmailAddress;</v>
       </c>
       <c r="G19" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="3:7">
       <c r="C20" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseConfirmYourTheParticipantsEmailAddress;</v>
       </c>
       <c r="G20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="3:7">
       <c r="C21" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseListYourTheParticipantsPhoneNumbersBelowAndIncludeCountryCode;</v>
       </c>
       <c r="G21" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="3:7">
       <c r="C22" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseAlsoSelectYourPreferredContactNumber;</v>
       </c>
       <c r="G22" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="3:7">
       <c r="C23" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D23" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
         <v>public String homePhoneNumber;</v>
       </c>
       <c r="G23" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="3:7">
       <c r="C24" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
         <v>public String workPhoneNumber;</v>
       </c>
       <c r="G24" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="3:7">
       <c r="C25" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D25" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
         <v>public String preferred;</v>
       </c>
       <c r="G25" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="3:7">
       <c r="C26" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
         <v>public String cellPhoneNumber;</v>
       </c>
       <c r="G26" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="3:7">
       <c r="C27" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D27" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
         <v>public String whatIsYourTheParticipantsRacePleaseSelectAllThatApply;</v>
       </c>
       <c r="G27" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="3:7">
       <c r="C28" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D28" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
         <v>public String whatIsYourTheParticipantsEthnicity;</v>
       </c>
       <c r="G28" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="3:7">
       <c r="C29" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
         <v>public String haveYouTheParticipantEverParticipatedInALiFraumeniSyndromeStudy;</v>
       </c>
       <c r="G29" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="3:7">
       <c r="C30" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
         <v>public String egAtAnotherMedicalInstitutionUniversityGovernmentAgencyOrOtherSite;</v>
       </c>
       <c r="G30" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="3:7">
       <c r="C31" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D31" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
         <v>public String pleaseSpecifyTheStudiesOrRegistryGroupsRegardingParticipationInOtherStudies;</v>
       </c>
       <c r="G31" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="32" spans="3:7">
       <c r="C32" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
         <v>public String doYouCurrentlyReceiveRegularLiFraumeniSyndromeScreeningOrManagement;</v>
       </c>
       <c r="G32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="3:7">
       <c r="C33" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
         <v>public String provideInformationAboutTheInstitutionWhereYou/theParticipantReceiveRegularLiFraumeniSyndromeManagement;</v>
       </c>
       <c r="G33" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="3:7">
       <c r="C34" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D34" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
         <v>public String physicianName;</v>
       </c>
       <c r="G34" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="3:7">
       <c r="C35" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D35" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
         <v>public String institutionName;</v>
       </c>
       <c r="G35" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="36" spans="3:7">
       <c r="C36" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
         <v>public String cityStateProvince;</v>
       </c>
       <c r="G36" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="3:7">
       <c r="C37" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D37" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E37" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
         <v>public String phoneNumber;</v>
       </c>
       <c r="G37" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="38" spans="3:7">
@@ -4647,7 +4857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46806D95-C0E7-034A-A2CD-2C82A125AC28}">
   <dimension ref="C2:H37"/>
   <sheetViews>
@@ -4665,728 +4875,728 @@
   <sheetData>
     <row r="2" spans="3:8">
       <c r="C2" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE(C2,D2,E2,F2)</f>
         <v>areYouCompletingThisQuestionnaireForSomeoneElse = testDataForMetforminScreener.get(MetforminScreenerConstants.ARE_YOU_COMPLETING_THIS_QUESTIONNAIRE_FOR_SOMEONE_ELSE);</v>
       </c>
       <c r="H2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="3:8">
       <c r="C3" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G17" si="0">CONCATENATE(C3,D3,E3,F3)</f>
         <v>whatIsYourName = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_NAME);</v>
       </c>
       <c r="H3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="3:8">
       <c r="C4" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>firstName = testDataForMetforminScreener.get(MetforminScreenerConstants.FIRST_NAME);</v>
       </c>
       <c r="H4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="3:8">
       <c r="C5" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>middleInitial = testDataForMetforminScreener.get(MetforminScreenerConstants.MIDDLE_INITIAL);</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="3:8">
       <c r="C6" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>lastName = testDataForMetforminScreener.get(MetforminScreenerConstants.LAST_NAME);</v>
       </c>
       <c r="H6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="3:8">
       <c r="C7" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
         <v>183</v>
-      </c>
-      <c r="D7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F7" t="s">
-        <v>186</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>theNextSetOfQuestionsWillCollectBasicInformationAboutYouTheParticipant = testDataForMetforminScreener.get(MetforminScreenerConstants.THE_NEXT_SET_OF_QUESTIONS_WILL_COLLECT_BASIC_INFORMATION_ABOUT_YOU_THE_PARTICIPANT);</v>
       </c>
       <c r="H7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="3:8">
       <c r="C8" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>whatIsYourTheParticipantsDateOfBirth = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANTS_DATE_OF_BIRTH);</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="3:8">
       <c r="C9" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>whatIsYouTheParticipantsSex = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANTS_SEX);</v>
       </c>
       <c r="H9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="3:8">
       <c r="C10" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>areYouTheParticipantAdopted = testDataForMetforminScreener.get(MetforminScreenerConstants.ARE_YOU_THE_PARTICIPANT_ADOPTED);</v>
       </c>
       <c r="H10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="3:8">
       <c r="C11" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>inWhichCountryDoYouTheParticipantCurrentlyLive = testDataForMetforminScreener.get(MetforminScreenerConstants.IN_WHICH_COUNTRY_DO_YOU_THE_PARTICIPANT_CURRENTLY_LIVE);</v>
       </c>
       <c r="H11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="3:8">
       <c r="C12" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>pleaseProvideTheMailingAddressWhereStudyMaterialsCanBeSentAsNeeded = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_PROVIDE_THE_MAILING_ADDRESS_WHERE_STUDY_MATERIALS_CAN_BE_SENT_AS_NEEDED);</v>
       </c>
       <c r="H12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="3:8">
       <c r="C13" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>street = testDataForMetforminScreener.get(MetforminScreenerConstants.STREET);</v>
       </c>
       <c r="H13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="3:8">
       <c r="C14" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>street2Optional = testDataForMetforminScreener.get(MetforminScreenerConstants.STREET_2_OPTIONAL);</v>
       </c>
       <c r="H14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="3:8">
       <c r="C15" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>city = testDataForMetforminScreener.get(MetforminScreenerConstants.CITY);</v>
       </c>
       <c r="H15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="3:8">
       <c r="C16" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>stateAbbreviation = testDataForMetforminScreener.get(MetforminScreenerConstants.STATE_ABBREVIATION);</v>
       </c>
       <c r="H16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="3:8">
       <c r="C17" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>zipCode = testDataForMetforminScreener.get(MetforminScreenerConstants.ZIP_CODE);</v>
       </c>
       <c r="H17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="3:8" s="19" customFormat="1"/>
     <row r="19" spans="3:8">
       <c r="C19" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G19" t="str">
         <f>CONCATENATE(C19,D19,E19,F19)</f>
         <v>whatIsYourTheParticipantsEmailAddress = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS);</v>
       </c>
       <c r="H19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="3:8">
       <c r="C20" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ref="G20:G36" si="1">CONCATENATE(C20,D20,E20,F20)</f>
         <v>pleaseConfirmYourTheParticipantsEmailAddress = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_CONFIRM_YOUR_THE_PARTICIPANTS_EMAIL_ADDRESS);</v>
       </c>
       <c r="H20" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="3:8">
       <c r="C21" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
         <v>pleaseListYourTheParticipantsPhoneNumbersBelowAndIncludeCountryCode = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_LIST_YOUR_THE_PARTICIPANTS_PHONE_NUMBERS_BELOW_AND_INCLUDE_COUNTRY_CODE);</v>
       </c>
       <c r="H21" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="3:8">
       <c r="C22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D22" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F22" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
         <v>pleaseAlsoSelectYourPreferredContactNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_ALSO_SELECT_YOUR_PREFERRED_CONTACT_NUMBER);</v>
       </c>
       <c r="H22" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="3:8">
       <c r="C23" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E23" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
         <v>homePhoneNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.HOME_PHONE_NUMBER);</v>
       </c>
       <c r="H23" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="3:8">
       <c r="C24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E24" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
         <v>workPhoneNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.WORK_PHONE_NUMBER);</v>
       </c>
       <c r="H24" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="3:8">
       <c r="C25" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E25" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F25" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
         <v>preferred = testDataForMetforminScreener.get(MetforminScreenerConstants.PREFERRED);</v>
       </c>
       <c r="H25" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="26" spans="3:8">
       <c r="C26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E26" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F26" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
         <v>cellPhoneNumber = testDataForMetforminScreener.get(MetforminScreenerConstants.CELL_PHONE_NUMBER);</v>
       </c>
       <c r="H26" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="3:8">
       <c r="C27" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E27" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
         <v>whatIsYourTheParticipantsRacePleaseSelectAllThatApply = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANT'S_RACE_PLEASE_SELECT_ALL_THAT_APPLY);</v>
       </c>
       <c r="H27" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="3:8">
       <c r="C28" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E28" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F28" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
         <v>whatIsYourTheParticipantsEthnicity = testDataForMetforminScreener.get(MetforminScreenerConstants.WHAT_IS_YOUR_THE_PARTICIPANT'S_ETHNICITY);</v>
       </c>
       <c r="H28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="3:8">
       <c r="C29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E29" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
         <v>haveYouTheParticipantEverParticipatedInALiFraumeniSyndromeStudy = testDataForMetforminScreener.get(MetforminScreenerConstants.HAVE_YOU_THE_PARTICIPANT_EVER_PARTICIPATED_IN_A_LIFRAUMENI_SYNDROME_STUDY);</v>
       </c>
       <c r="H29" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="3:8">
       <c r="C30" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D30" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E30" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
         <v>egAtAnotherMedicalInstitutionUniversityGovernmentAgencyOrOtherSite = testDataForMetforminScreener.get(MetforminScreenerConstants.EG_AT_ANOTHER_MEDICAL_INSTITUTION_UNIVERSITY_GOVERNMENT_AGENCY_OR_OTHER_SITE);</v>
       </c>
       <c r="H30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="3:8">
       <c r="C31" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E31" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F31" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
         <v>pleaseSpecifyTheStudiesOrRegistryGroupsRegardingParticipationInOtherStudies = testDataForMetforminScreener.get(MetforminScreenerConstants.PLEASE_SPECIFY_THE_STUDYIES_OR_REGISTRY_GROUPS_REGARDING_PARTICIPATION_IN_OTHER_STUDIES);</v>
       </c>
       <c r="H31" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="3:8">
       <c r="C32" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E32" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
         <v>doYouCurrentlyReceiveRegularLiFraumeniSyndromeScreeningOrManagement = testDataForMetforminScreener.get(MetforminScreenerConstants.DO_YOU_CURRENTLY_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_SCREENING_OR_MANAGEMENT);</v>
       </c>
       <c r="H32" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="3:8">
       <c r="C33" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D33" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E33" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
         <v>provideInformationAboutTheInstitutionWhereYou/theParticipantReceiveRegularLiFraumeniSyndromeManagement = testDataForMetforminScreener.get(MetforminScreenerConstants.PROVIDE_INFORMATION_ABOUT_THE_INSTITUTION_WHERE_YOU_THE_PARTICIPANT_RECEIVE_REGULAR_LIFRAUMENI_SYNDROME_MANAGEMENT);</v>
       </c>
       <c r="H33" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="3:8">
       <c r="C34" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E34" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
         <v>physicianName = testDataForMetforminScreener.get(MetforminScreenerConstants.PHYSICIAN_NAME);</v>
       </c>
       <c r="H34" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="35" spans="3:8">
       <c r="C35" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E35" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
         <v>institutionName = testDataForMetforminScreener.get(MetforminScreenerConstants.INSTITUTION_NAME);</v>
       </c>
       <c r="H35" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="3:8">
       <c r="C36" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E36" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F36" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
         <v>cityStateProvince = testDataForMetforminScreener.get(MetforminScreenerConstants.CITY_STATE_PROVINCE);</v>
       </c>
       <c r="H36" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="3:8">
       <c r="C37" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D37" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E37" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -5395,7 +5605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD1CF35-4A95-4849-A40C-678131F58510}">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added the Medical and Final Questions tab assertion in Referral page of NV for Metformin
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
+++ b/src/test/java/CHARMS/resources/MetforminScreenerData.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE0CA8-DBD4-BF41-A6F8-FF79E32A534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359D235E-3955-9442-AD70-710223568CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17640" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
     <sheet name="MetforminScreenerScenario1" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
-    <sheet name="Sheet8" sheetId="11" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet9" sheetId="12" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="8" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="9" r:id="rId7"/>
-    <sheet name="MetforminScreenerScenario2" sheetId="5" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="15" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="14" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId4"/>
+    <sheet name="Sheet8" sheetId="11" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet9" sheetId="12" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="9" r:id="rId9"/>
+    <sheet name="MetforminScreenerScenario2" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="487">
   <si>
     <t>Yes</t>
   </si>
@@ -1418,12 +1420,695 @@
   <si>
     <t>work_phone</t>
   </si>
+  <si>
+    <r>
+      <t>CharmsUtil.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>assertTextBoxData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>softAssert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreenerPage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.dynamicLocatorForInputElementsOfFamily(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>"state"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreener_TestDataManager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>stateAbbreviation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>" State/Province Value of the Contact Information in  Fanconi Study screener page "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CharmsUtil.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>assertDropDownData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>softAssert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreenerPage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.dynamicLocatorForSelectElement(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>"legal_guardian"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreener_TestDataManager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>areYouTheLegalGuardianOfThisPerson</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>" Relationship Value of the Contact Info on Fanconi Study Screener page "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CharmsUtil.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>assertDropDownData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>softAssert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreenerPage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.dynamicLocatorForSelectElement(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>"relationship"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreener_TestDataManager</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>whatIsYourRelationshipToParticipant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>" Relationship Value of the Contact Info on Fanconi Study Screener page "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CharmsUtil.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>assertTextBoxData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>softAssert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>metforminScreenerPage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.dynamicLocatorForInputElementsOfFamily(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>"proxy_state"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>" State/Province Value of the Contact Information in  Fanconi Study screener page "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan(MetforminScreenerConstants.FIRST_NAME), MetforminScreenerConstants.FIRST_NAME, " First Name label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("first_name"), metforminScreener_TestDataManager.firstName, " First Name Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan(MetforminScreenerConstants.MIDDLE_NAME), MetforminScreenerConstants.MIDDLE_NAME, " Middle Name label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("middle_name"), metforminScreener_TestDataManager.middleInitial, " Middle Name Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan(MetforminScreenerConstants.LAST_NAME), MetforminScreenerConstants.LAST_NAME, " Last Name label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("last_name"), metforminScreener_TestDataManager.lastName, " Last Name Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan(MetforminScreenerConstants.IN_WHICH_COUNTRY_DO_YOU_THE_PARTICIPANT_CURRENTLY_LIVE), MetforminScreenerConstants.IN_WHICH_COUNTRY_DO_YOU_THE_PARTICIPANT_CURRENTLY_LIVE, " Contact Country label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForDisplayReadOnlyInputElements("country"), metforminScreener_TestDataManager.inWhichCountryDoYouTheParticipantCurrentlyLive, " Contact Country Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Street Address"), "Street Address", " Street Address label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("street_address"), metforminScreener_TestDataManager.street, " Street Address Value for non USA country of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Street 2 (optional)"), "Street 2 (optional)", " Street 2 (optional) label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("street_address2"), metforminScreener_TestDataManager.street2Optional, " Street 2 (optional) Value for non USA country of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("City"), "City", " City label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("city"), metforminScreener_TestDataManager.city, " City Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("State/Province"), "State/Province", " State/Province label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Zip Code"), "Zip Code", " Zip Code label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("zip_code"), metforminScreener_TestDataManager.zipCode, " Contact Zip Code Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Email Address"), "Email Address", " Email Address label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("email_address"), metforminScreener_TestDataManager.whatIsYourTheParticipantsEmailAddress, " Contact Email Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Preferred Contact"), "Preferred Contact", " Preferred Contact label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForSelectElement("preferred_contact"), metforminScreener_TestDataManager.preferredContact, " Preferred Contact Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Home Phone Number"), "Home Phone Number", " Home Phone Number label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("home_phone"), metforminScreener_TestDataManager.homePhoneNumber, " Contact Home Phone Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Cell Phone Number"), "Cell Phone Number", " Cell Phone Number label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("cell_phone"), metforminScreener_TestDataManager.cellPhoneNumber, " Cell Phone Number Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Work Phone Number"), "Work Phone Number", " Work Phone Number label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("work_phone"), metforminScreener_TestDataManager.workPhoneNumber, " Work Phone Number Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan(MetforminScreenerConstants.ARE_YOU_THE_LEGAL_GUARDIAN_OF_THIS_PERSON), "Are you the legal guardian of this person?", " Are you the legal guardian of this person? label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("What is your relationship to this person?"), "What is your relationship to this person?", " What is your relationship to this person? label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy First Name"), "Proxy First Name", " Proxy First Name label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("your_first_name"), metforminScreener_TestDataManager.proxyFirstName, " Proxy First Name  Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Middle Name"), "Proxy Middle Name", " Proxy Middle Name label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("your_middle_name"), metforminScreener_TestDataManager.proxyMiddleName, " Proxy Middle Name Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Last Name"), "Proxy Last Name", " Proxy Last Name label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("your_last_name"), metforminScreener_TestDataManager.proxyLastName, " Proxy Last Name Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Street Address"), "Proxy Street Address", " Proxy Street Address label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_street_address"), "", " Street Address Value for non USA country of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Street Address 2 (Optional)"), "Proxy Street Address 2 (Optional)", " Proxy Street Address 2 (Optional) label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_street_address_2"), "", " Proxy Street Address 2 (Optional) Value for non USA country of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy City"), "Proxy City", " Proxy City label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_city"), "", " Proxy City Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy State/Province"), "Proxy State/Province", " Proxy State/Province label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Zip Code"), "Proxy Zip Code", " Proxy Zip Code label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_zip_code"), "", " Proxy Zip Code Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Email Address"), "Proxy Email Address", " Proxy Email Address label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_email_address"), "", " Proxy Email Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Home Phone"), "Proxy Home Phone", " Proxy Home Phone label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_home_phone"), "", " Proxy Home Phone Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Cell Phone"), "Proxy Cell Phone", " Proxy Cell Phone label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorForInputElementsOfFamily("proxy_cell_phone"), "", " Proxy Cell Phone Value of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>CharmsUtil.assertTextBoxData(softAssert, metforminScreenerPage.dynamicLocatorUsingNormalizeSpaceInSpan("Proxy Work Phone"), "Proxy Work Phone", " Proxy Work Phone label of the Contact Information tab in Metformin Referral page ");</t>
+  </si>
+  <si>
+    <t>When did you/the participant stop taking Metformin?</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>-- None --</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1460,6 +2145,38 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFC77DBB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFC77DBB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF151920"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1503,7 +2220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1558,6 +2275,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1582,6 +2306,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>121060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BACD85F-6F93-E347-4B55-3626C9869F69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5778500" y="1016000"/>
+          <a:ext cx="7772400" cy="3981860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1881,10 +2654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BDBA15-09FD-FB42-B4F3-2AA9D176499A}">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2328,175 +3101,175 @@
     </row>
     <row r="59" spans="1:2" ht="19">
       <c r="A59" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>485</v>
+      </c>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" ht="19">
       <c r="A60" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B60" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="61" spans="1:2" ht="19">
       <c r="A61" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="B61" s="5">
-        <v>103</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2" ht="19">
       <c r="A62" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="B62" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="B62" s="5">
+        <v>103</v>
+      </c>
     </row>
     <row r="63" spans="1:2" ht="19">
       <c r="A63" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="B63" s="5"/>
+        <v>389</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="64" spans="1:2" ht="19">
       <c r="A64" s="11" t="s">
-        <v>79</v>
+        <v>390</v>
       </c>
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="1:2" ht="19">
       <c r="A65" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" ht="19">
       <c r="A66" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19">
       <c r="A67" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B67" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="68" spans="1:2" ht="19">
       <c r="A68" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>85</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B68" s="5"/>
     </row>
     <row r="69" spans="1:2" ht="19">
       <c r="A69" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="19">
       <c r="A70" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="19">
       <c r="A71" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B71" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="72" spans="1:2" ht="19">
       <c r="A72" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:2" ht="19">
       <c r="A73" s="11" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="19">
       <c r="A74" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>386</v>
+        <v>91</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="19">
       <c r="A75" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="19">
       <c r="A76" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>387</v>
+        <v>93</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="19">
       <c r="A77" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>0</v>
+        <v>376</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="19">
       <c r="A78" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B78" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:2" ht="19">
       <c r="A79" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" ht="19">
       <c r="A80" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B80" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="81" spans="1:2" ht="19">
       <c r="A81" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" ht="19">
       <c r="A82" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>0</v>
@@ -2504,286 +3277,674 @@
     </row>
     <row r="83" spans="1:2" ht="19">
       <c r="A83" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="38">
+    <row r="84" spans="1:2" ht="19">
       <c r="A84" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="38">
+      <c r="A85" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B84" s="4"/>
-    </row>
-    <row r="85" spans="1:2" ht="19">
-      <c r="A85" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" ht="19">
       <c r="A86" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="18">
+      <c r="A87" s="23" t="s">
+        <v>484</v>
+      </c>
+      <c r="B87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" ht="19">
+      <c r="A88" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B86" s="4"/>
-    </row>
-    <row r="87" spans="1:2" ht="19">
-      <c r="A87" s="11" t="s">
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" spans="1:2" ht="19">
+      <c r="A89" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="76">
-      <c r="A88" s="11" t="s">
+    <row r="90" spans="1:2" ht="76">
+      <c r="A90" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="95">
-      <c r="A89" s="11" t="s">
+    <row r="91" spans="1:2" ht="95">
+      <c r="A91" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="19">
-      <c r="A90" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="19">
-      <c r="A91" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="19">
       <c r="A92" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="B92" s="4">
-        <v>1234356758</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="38">
+        <v>109</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="19">
       <c r="A93" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="19">
       <c r="A94" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="19">
+        <v>378</v>
+      </c>
+      <c r="B94" s="4">
+        <v>1234356758</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="38">
       <c r="A95" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B95" s="4"/>
+        <v>113</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:2" ht="19">
       <c r="A96" s="11" t="s">
-        <v>379</v>
+        <v>114</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="38">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="19">
       <c r="A97" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>116</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B97" s="4"/>
     </row>
     <row r="98" spans="1:2" ht="19">
       <c r="A98" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="38">
+      <c r="A99" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="19">
+      <c r="A100" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B98" s="4"/>
-    </row>
-    <row r="99" spans="1:2" ht="76">
-      <c r="A99" s="11" t="s">
+      <c r="B100" s="4"/>
+    </row>
+    <row r="101" spans="1:2" ht="76">
+      <c r="A101" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="95">
-      <c r="A100" s="11" t="s">
+    <row r="102" spans="1:2" ht="95">
+      <c r="A102" s="11" t="s">
         <v>392</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="57">
-      <c r="A101" s="11" t="s">
+    <row r="103" spans="1:2" ht="57">
+      <c r="A103" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>397</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="19">
-      <c r="A102" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="19">
-      <c r="A103" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="19">
       <c r="A104" s="11" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>0</v>
+        <v>394</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="19">
       <c r="A105" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="B105" s="4"/>
+        <v>403</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="106" spans="1:2" ht="19">
       <c r="A106" s="11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>410</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="19">
       <c r="A107" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="B107" s="14" t="s">
-        <v>405</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="B107" s="4"/>
     </row>
     <row r="108" spans="1:2" ht="19">
       <c r="A108" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>401</v>
+        <v>409</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="19">
       <c r="A109" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="B109" s="5"/>
+        <v>402</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="110" spans="1:2" ht="19">
       <c r="A110" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="B110" s="5"/>
+        <v>400</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="111" spans="1:2" ht="19">
       <c r="A111" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B111" s="5"/>
     </row>
     <row r="112" spans="1:2" ht="19">
       <c r="A112" s="11" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B112" s="5"/>
     </row>
     <row r="113" spans="1:2" ht="19">
       <c r="A113" s="11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B113" s="5"/>
     </row>
     <row r="114" spans="1:2" ht="19">
       <c r="A114" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="B114" s="15"/>
+        <v>418</v>
+      </c>
+      <c r="B114" s="5"/>
     </row>
     <row r="115" spans="1:2" ht="19">
       <c r="A115" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="B115" s="15"/>
+        <v>419</v>
+      </c>
+      <c r="B115" s="5"/>
     </row>
     <row r="116" spans="1:2" ht="19">
       <c r="A116" s="11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B116" s="15"/>
     </row>
     <row r="117" spans="1:2" ht="19">
       <c r="A117" s="11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B117" s="15"/>
     </row>
     <row r="118" spans="1:2" ht="19">
       <c r="A118" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B118" s="15"/>
     </row>
     <row r="119" spans="1:2" ht="19">
       <c r="A119" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B119" s="15"/>
     </row>
     <row r="120" spans="1:2" ht="19">
       <c r="A120" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="B120" s="15"/>
+    </row>
+    <row r="121" spans="1:2" ht="19">
+      <c r="A121" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="B121" s="15"/>
+    </row>
+    <row r="122" spans="1:2" ht="19">
+      <c r="A122" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="B122" s="11" t="s">
         <v>428</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B106" r:id="rId1" xr:uid="{79ECE5D9-FE27-534A-9CE9-220483AFFCAE}"/>
+    <hyperlink ref="B108" r:id="rId1" xr:uid="{79ECE5D9-FE27-534A-9CE9-220483AFFCAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD1CF35-4A95-4849-A40C-678131F58510}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" ht="18">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5ED1CA9-44B9-D845-B149-79AB83C0E1FC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD480A77-4FF5-0943-8951-B699FCFD969F}">
+  <dimension ref="E2:E56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="5" max="5" width="115.1640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:5" ht="29">
+      <c r="E2" s="22" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="5:5" ht="29">
+      <c r="E3" s="22" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5" ht="29">
+      <c r="E4" s="22" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="5:5" ht="29">
+      <c r="E5" s="22" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="5:5" ht="29">
+      <c r="E6" s="22" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7" spans="5:5" ht="29">
+      <c r="E7" s="22" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" ht="57">
+      <c r="E8" s="22" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="5:5" ht="43">
+      <c r="E9" s="22" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="5:5" ht="29">
+      <c r="E10" s="22" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5" ht="29">
+      <c r="E11" s="22" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5" ht="29">
+      <c r="E12" s="22" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5" ht="29">
+      <c r="E13" s="22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" ht="29">
+      <c r="E14" s="22" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" ht="29">
+      <c r="E15" s="22" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" ht="29">
+      <c r="E16" s="22" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" ht="29">
+      <c r="E17" s="22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" ht="29">
+      <c r="E18" s="22" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" ht="29">
+      <c r="E19" s="22" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" ht="29">
+      <c r="E20" s="22" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" ht="29">
+      <c r="E21" s="22" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" ht="29">
+      <c r="E22" s="22" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" ht="29">
+      <c r="E23" s="22" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" ht="29">
+      <c r="E24" s="22" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" ht="29">
+      <c r="E25" s="22" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" ht="29">
+      <c r="E26" s="22" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" ht="29">
+      <c r="E27" s="22" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" ht="29">
+      <c r="E28" s="22" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" ht="29">
+      <c r="E29" s="22" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" ht="43">
+      <c r="E30" s="22" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" ht="29">
+      <c r="E31" s="22" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" ht="29">
+      <c r="E32" s="22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" ht="29">
+      <c r="E33" s="22" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" ht="29">
+      <c r="E34" s="22" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" ht="29">
+      <c r="E35" s="22" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" ht="29">
+      <c r="E36" s="22" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" ht="29">
+      <c r="E37" s="22" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" ht="29">
+      <c r="E38" s="22" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" ht="29">
+      <c r="E39" s="22" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" ht="29">
+      <c r="E40" s="22" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" ht="29">
+      <c r="E41" s="22" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" ht="29">
+      <c r="E42" s="22" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" ht="29">
+      <c r="E43" s="22" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" ht="29">
+      <c r="E44" s="22" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" ht="29">
+      <c r="E45" s="22" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" ht="29">
+      <c r="E46" s="22" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" ht="29">
+      <c r="E47" s="22" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5" ht="29">
+      <c r="E48" s="22" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" ht="29">
+      <c r="E49" s="22" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" ht="29">
+      <c r="E50" s="22" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" ht="29">
+      <c r="E51" s="22" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" ht="29">
+      <c r="E52" s="22" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" ht="29">
+      <c r="E53" s="22" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" ht="29">
+      <c r="E54" s="22" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" ht="29">
+      <c r="E55" s="22" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" ht="29">
+      <c r="E56" s="22" t="s">
+        <v>483</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89481F3-DE1D-084D-8820-B9A4FEFE8064}">
   <dimension ref="F3:F4"/>
   <sheetViews>
@@ -2801,7 +3962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="6:6" ht="152">
+    <row r="4" spans="6:6" ht="19">
       <c r="F4" s="11" t="s">
         <v>27</v>
       </c>
@@ -2811,7 +3972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8893135-DC7A-C241-A6F6-938ADF884C45}">
   <dimension ref="E2:E81"/>
   <sheetViews>
@@ -3224,7 +4385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3BD33-B5B5-034F-9377-39C67236667B}">
   <dimension ref="C2:I51"/>
   <sheetViews>
@@ -4171,7 +5332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D26075-03E2-6D49-B34D-6A66EA88B4F3}">
   <dimension ref="G2:H2"/>
   <sheetViews>
@@ -4194,7 +5355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6723C2-64BA-2E4A-9742-DB943F1C4B65}">
   <dimension ref="C2:G38"/>
   <sheetViews>
@@ -4857,7 +6018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46806D95-C0E7-034A-A2CD-2C82A125AC28}">
   <dimension ref="C2:H37"/>
   <sheetViews>
@@ -5603,69 +6764,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD1CF35-4A95-4849-A40C-678131F58510}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="62.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" ht="18">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>